<commit_message>
Seperated in 3 files - all on Dataset df only
</commit_message>
<xml_diff>
--- a/Customer_Satisfaction_Capstone/StateOrder.xlsx
+++ b/Customer_Satisfaction_Capstone/StateOrder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravindranadh.y.ITLINFOSYS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravin\Documents\GitHub\Projects\Customer_Satisfaction_Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,9 +92,6 @@
     <t>west bengal</t>
   </si>
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>OrderState</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>01tamil nadu</t>
+  </si>
+  <si>
+    <t>StateCorrected</t>
   </si>
 </sst>
 </file>
@@ -500,9 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -512,10 +510,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -523,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -539,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +569,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -587,7 +585,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -603,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -611,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -619,7 +617,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -627,7 +625,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,7 +633,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +649,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +657,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +665,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -675,7 +673,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -683,7 +681,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -691,7 +689,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>